<commit_message>
tampilan web yang bisa diakses
website dengan prediksi nyata yang tak buat ketika PA1, sudah nyambung ke db. evaluasi belum nyambung ke websitenya
</commit_message>
<xml_diff>
--- a/pa1/rangkuman_evaluasi_multi_output.xlsx
+++ b/pa1/rangkuman_evaluasi_multi_output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PA lintang\PandasApp\pa1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratih\Documents\GitHub\TA-lintang\pa1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0004495-625B-4FAD-9C5C-792110BD44FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FCC889-4962-4A0F-8B2B-8A54E7648AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -679,12 +679,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -723,17 +729,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,7 +1075,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -1088,7 +1095,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1106,7 +1113,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -1119,12 +1126,12 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1149,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
@@ -1162,7 +1169,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -1180,7 +1187,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1198,7 +1205,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1216,7 +1223,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B10" t="s">
@@ -1236,7 +1243,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +1261,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -1272,7 +1279,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -1290,7 +1297,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B14" t="s">
@@ -1310,7 +1317,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1335,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -1346,7 +1353,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1364,7 +1371,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B18" t="s">
@@ -1384,7 +1391,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1402,7 +1409,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -1415,12 +1422,12 @@
       <c r="E20" t="s">
         <v>89</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="2"/>
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -1438,7 +1445,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B22" t="s">
@@ -1458,7 +1465,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="2"/>
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -1476,7 +1483,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -1494,7 +1501,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="2"/>
       <c r="B25" t="s">
         <v>22</v>
       </c>
@@ -1512,7 +1519,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B26" t="s">
@@ -1532,7 +1539,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -1550,7 +1557,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -1568,7 +1575,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="2"/>
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1586,7 +1593,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B30" t="s">
@@ -1606,7 +1613,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="2"/>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1631,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="2"/>
       <c r="B32" t="s">
         <v>17</v>
       </c>
@@ -1642,7 +1649,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="2"/>
       <c r="B33" t="s">
         <v>22</v>
       </c>
@@ -1660,7 +1667,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B34" t="s">
@@ -1680,7 +1687,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="2"/>
       <c r="B35" t="s">
         <v>12</v>
       </c>
@@ -1698,7 +1705,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="2"/>
       <c r="B36" t="s">
         <v>17</v>
       </c>
@@ -1716,7 +1723,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="2"/>
       <c r="B37" t="s">
         <v>22</v>
       </c>
@@ -1734,7 +1741,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B38" t="s">
@@ -1754,7 +1761,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="2"/>
       <c r="B39" t="s">
         <v>12</v>
       </c>
@@ -1772,7 +1779,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="2"/>
       <c r="B40" t="s">
         <v>17</v>
       </c>
@@ -1790,7 +1797,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="2"/>
       <c r="B41" t="s">
         <v>22</v>
       </c>
@@ -1808,7 +1815,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B42" t="s">
@@ -1828,7 +1835,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="2"/>
       <c r="B43" t="s">
         <v>12</v>
       </c>
@@ -1846,7 +1853,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="2"/>
       <c r="B44" t="s">
         <v>17</v>
       </c>
@@ -1859,12 +1866,12 @@
       <c r="E44" t="s">
         <v>190</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="4" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="2"/>
       <c r="B45" t="s">
         <v>22</v>
       </c>
@@ -1882,7 +1889,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B46" t="s">
@@ -1902,7 +1909,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="2"/>
       <c r="B47" t="s">
         <v>12</v>
       </c>
@@ -1920,7 +1927,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
+      <c r="A48" s="2"/>
       <c r="B48" t="s">
         <v>17</v>
       </c>
@@ -1938,7 +1945,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="2"/>
       <c r="B49" t="s">
         <v>22</v>
       </c>
@@ -1957,11 +1964,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
@@ -1969,6 +1971,11 @@
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A45"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>